<commit_message>
New bayesian script and stan model
</commit_message>
<xml_diff>
--- a/Cook_Inlet/Kenai Sockeye/Hasbrouck 2022 kenai late run sockeye data.xlsx
+++ b/Cook_Inlet/Kenai Sockeye/Hasbrouck 2022 kenai late run sockeye data.xlsx
@@ -1,25 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20416"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\richard.brenner\Desktop\Cook Inlet TEMP\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aaron.lambert\Documents\Cook-Inlet-SAFE\Cook_Inlet\Kenai Sockeye\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{496164CE-1371-4F87-A96C-F7A00EC0CDB4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="12" windowWidth="18960" windowHeight="11328"/>
+    <workbookView xWindow="120" yWindow="15" windowWidth="18960" windowHeight="11325" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Table 1" sheetId="1" r:id="rId1"/>
+    <sheet name="Full Series" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
   <si>
     <r>
       <rPr>
@@ -100,11 +102,14 @@
       <t>Harvest</t>
     </r>
   </si>
+  <si>
+    <t>Run</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
@@ -366,6 +371,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -401,6 +423,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -576,26 +615,26 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="E54" sqref="E54"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="G1" sqref="G1:G52"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="9.33203125" customWidth="1"/>
-    <col min="2" max="2" width="15.109375" customWidth="1"/>
+    <col min="2" max="2" width="15.1640625" customWidth="1"/>
     <col min="3" max="3" width="14" customWidth="1"/>
     <col min="4" max="4" width="9.33203125" customWidth="1"/>
-    <col min="5" max="5" width="11.5546875" customWidth="1"/>
-    <col min="6" max="6" width="15.109375" customWidth="1"/>
+    <col min="5" max="5" width="11.5" customWidth="1"/>
+    <col min="6" max="6" width="15.1640625" customWidth="1"/>
     <col min="7" max="7" width="12.6640625" customWidth="1"/>
-    <col min="8" max="8" width="11.5546875" customWidth="1"/>
+    <col min="8" max="8" width="11.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -621,7 +660,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="5">
         <v>1968</v>
       </c>
@@ -643,7 +682,7 @@
       <c r="G2" s="10"/>
       <c r="H2" s="10"/>
     </row>
-    <row r="3" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="11">
         <v>1969</v>
       </c>
@@ -665,7 +704,7 @@
       <c r="G3" s="16"/>
       <c r="H3" s="16"/>
     </row>
-    <row r="4" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="11">
         <v>1970</v>
       </c>
@@ -687,7 +726,7 @@
       <c r="G4" s="16"/>
       <c r="H4" s="16"/>
     </row>
-    <row r="5" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="11">
         <v>1971</v>
       </c>
@@ -709,7 +748,7 @@
       <c r="G5" s="16"/>
       <c r="H5" s="16"/>
     </row>
-    <row r="6" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="11">
         <v>1972</v>
       </c>
@@ -731,7 +770,7 @@
       <c r="G6" s="16"/>
       <c r="H6" s="16"/>
     </row>
-    <row r="7" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="11">
         <v>1973</v>
       </c>
@@ -753,7 +792,7 @@
       <c r="G7" s="16"/>
       <c r="H7" s="16"/>
     </row>
-    <row r="8" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="11">
         <v>1974</v>
       </c>
@@ -775,7 +814,7 @@
       <c r="G8" s="16"/>
       <c r="H8" s="16"/>
     </row>
-    <row r="9" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="11">
         <v>1975</v>
       </c>
@@ -801,7 +840,7 @@
         <v>301088</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="11">
         <v>1976</v>
       </c>
@@ -827,7 +866,7 @@
         <v>867167</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="11">
         <v>1977</v>
       </c>
@@ -853,7 +892,7 @@
         <v>1317529</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="11">
         <v>1978</v>
       </c>
@@ -879,7 +918,7 @@
         <v>1584561</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="18">
         <v>1979</v>
       </c>
@@ -905,7 +944,7 @@
         <v>424028</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="18">
         <v>1980</v>
       </c>
@@ -931,7 +970,7 @@
         <v>866012</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="18">
         <v>1981</v>
       </c>
@@ -957,7 +996,7 @@
         <v>640886</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="18">
         <v>1982</v>
       </c>
@@ -983,7 +1022,7 @@
         <v>2010770</v>
       </c>
     </row>
-    <row r="17" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="18">
         <v>1983</v>
       </c>
@@ -1009,7 +1048,7 @@
         <v>3188646</v>
       </c>
     </row>
-    <row r="18" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="18">
         <v>1984</v>
       </c>
@@ -1035,7 +1074,7 @@
         <v>840381</v>
       </c>
     </row>
-    <row r="19" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="18">
         <v>1985</v>
       </c>
@@ -1061,7 +1100,7 @@
         <v>1922255</v>
       </c>
     </row>
-    <row r="20" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="18">
         <v>1986</v>
       </c>
@@ -1087,7 +1126,7 @@
         <v>2390754</v>
       </c>
     </row>
-    <row r="21" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="18">
         <v>1987</v>
       </c>
@@ -1113,7 +1152,7 @@
         <v>7380239</v>
       </c>
     </row>
-    <row r="22" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="18">
         <v>1988</v>
       </c>
@@ -1139,7 +1178,7 @@
         <v>4841654</v>
       </c>
     </row>
-    <row r="23" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="18">
         <v>1989</v>
       </c>
@@ -1165,7 +1204,7 @@
         <v>4629655</v>
       </c>
     </row>
-    <row r="24" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="18">
         <v>1990</v>
       </c>
@@ -1191,7 +1230,7 @@
         <v>2429567</v>
       </c>
     </row>
-    <row r="25" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="18">
         <v>1991</v>
       </c>
@@ -1217,7 +1256,7 @@
         <v>1454936</v>
       </c>
     </row>
-    <row r="26" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="18">
         <v>1992</v>
       </c>
@@ -1243,7 +1282,7 @@
         <v>7027916</v>
       </c>
     </row>
-    <row r="27" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="18">
         <v>1993</v>
       </c>
@@ -1269,7 +1308,7 @@
         <v>3448502</v>
       </c>
     </row>
-    <row r="28" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="18">
         <v>1994</v>
       </c>
@@ -1295,7 +1334,7 @@
         <v>2577249</v>
       </c>
     </row>
-    <row r="29" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="18">
         <v>1995</v>
       </c>
@@ -1321,7 +1360,7 @@
         <v>1851708</v>
       </c>
     </row>
-    <row r="30" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="18">
         <v>1996</v>
       </c>
@@ -1347,7 +1386,7 @@
         <v>2732959</v>
       </c>
     </row>
-    <row r="31" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="18">
         <v>1997</v>
       </c>
@@ -1373,7 +1412,7 @@
         <v>3244366</v>
       </c>
     </row>
-    <row r="32" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="18">
         <v>1998</v>
       </c>
@@ -1399,7 +1438,7 @@
         <v>973129</v>
       </c>
     </row>
-    <row r="33" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="18">
         <v>1999</v>
       </c>
@@ -1425,7 +1464,7 @@
         <v>2035292</v>
       </c>
     </row>
-    <row r="34" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="18">
         <v>2000</v>
       </c>
@@ -1451,7 +1490,7 @@
         <v>1117880</v>
       </c>
     </row>
-    <row r="35" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="18">
         <v>2001</v>
       </c>
@@ -1477,7 +1516,7 @@
         <v>1451441</v>
       </c>
     </row>
-    <row r="36" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="18">
         <v>2002</v>
       </c>
@@ -1503,7 +1542,7 @@
         <v>2340146</v>
       </c>
     </row>
-    <row r="37" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="18">
         <v>2003</v>
       </c>
@@ -1529,7 +1568,7 @@
         <v>3037279</v>
       </c>
     </row>
-    <row r="38" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="18">
         <v>2004</v>
       </c>
@@ -1555,7 +1594,7 @@
         <v>4014594</v>
       </c>
     </row>
-    <row r="39" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="18">
         <v>2005</v>
       </c>
@@ -1581,7 +1620,7 @@
         <v>4455170</v>
       </c>
     </row>
-    <row r="40" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="18">
         <v>2006</v>
       </c>
@@ -1607,7 +1646,7 @@
         <v>956507</v>
       </c>
     </row>
-    <row r="41" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="18">
         <v>2007</v>
       </c>
@@ -1633,7 +1672,7 @@
         <v>2637535</v>
       </c>
     </row>
-    <row r="42" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="18">
         <v>2008</v>
       </c>
@@ -1659,7 +1698,7 @@
         <v>1373626</v>
       </c>
     </row>
-    <row r="43" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="18">
         <v>2009</v>
       </c>
@@ -1685,7 +1724,7 @@
         <v>1582297</v>
       </c>
     </row>
-    <row r="44" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="18">
         <v>2010</v>
       </c>
@@ -1711,7 +1750,7 @@
         <v>2558156</v>
       </c>
     </row>
-    <row r="45" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="18">
         <v>2011</v>
       </c>
@@ -1737,7 +1776,7 @@
         <v>4982359</v>
       </c>
     </row>
-    <row r="46" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="18">
         <v>2012</v>
       </c>
@@ -1763,7 +1802,7 @@
         <v>3556760</v>
       </c>
     </row>
-    <row r="47" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="18">
         <v>2013</v>
       </c>
@@ -1781,7 +1820,7 @@
         <v>2647914</v>
       </c>
     </row>
-    <row r="48" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="18">
         <v>2014</v>
       </c>
@@ -1799,7 +1838,7 @@
         <v>2185693</v>
       </c>
     </row>
-    <row r="49" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="18">
         <v>2015</v>
       </c>
@@ -1817,7 +1856,7 @@
         <v>2418696</v>
       </c>
     </row>
-    <row r="50" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="18">
         <v>2016</v>
       </c>
@@ -1835,7 +1874,7 @@
         <v>2593688</v>
       </c>
     </row>
-    <row r="51" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="18">
         <v>2017</v>
       </c>
@@ -1853,7 +1892,7 @@
         <v>1538947</v>
       </c>
     </row>
-    <row r="52" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="25">
         <v>2018</v>
       </c>
@@ -1874,4 +1913,434 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43B6890C-0BFD-4EC4-9336-5D3966886CF2}">
+  <dimension ref="A1:B53"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K21" sqref="K21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" s="11">
+        <v>1975</v>
+      </c>
+      <c r="B2">
+        <v>485350</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" s="11">
+        <v>1976</v>
+      </c>
+      <c r="B3">
+        <v>1374607</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" s="11">
+        <v>1977</v>
+      </c>
+      <c r="B4">
+        <v>2268567</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" s="11">
+        <v>1978</v>
+      </c>
+      <c r="B5">
+        <v>2096342</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" s="18">
+        <v>1979</v>
+      </c>
+      <c r="B6">
+        <v>797838</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" s="18">
+        <v>1980</v>
+      </c>
+      <c r="B7">
+        <v>1481394</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" s="18">
+        <v>1981</v>
+      </c>
+      <c r="B8">
+        <v>1176410</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" s="18">
+        <v>1982</v>
+      </c>
+      <c r="B9">
+        <v>2766442</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" s="18">
+        <v>1983</v>
+      </c>
+      <c r="B10">
+        <v>3981411</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" s="18">
+        <v>1984</v>
+      </c>
+      <c r="B11">
+        <v>1286678</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" s="18">
+        <v>1985</v>
+      </c>
+      <c r="B12">
+        <v>2496016</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13" s="18">
+        <v>1986</v>
+      </c>
+      <c r="B13">
+        <v>2945961</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A14" s="18">
+        <v>1987</v>
+      </c>
+      <c r="B14">
+        <v>9391896</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A15" s="18">
+        <v>1988</v>
+      </c>
+      <c r="B15">
+        <v>6054519</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A16" s="18">
+        <v>1989</v>
+      </c>
+      <c r="B16">
+        <v>6656274</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" s="18">
+        <v>1990</v>
+      </c>
+      <c r="B17">
+        <v>3224183</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18" s="18">
+        <v>1991</v>
+      </c>
+      <c r="B18">
+        <v>2182082</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19" s="18">
+        <v>1992</v>
+      </c>
+      <c r="B19">
+        <v>8235298</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A20" s="18">
+        <v>1993</v>
+      </c>
+      <c r="B20">
+        <v>4446195</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A21" s="18">
+        <v>1994</v>
+      </c>
+      <c r="B21">
+        <v>3886918</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A22" s="18">
+        <v>1995</v>
+      </c>
+      <c r="B22">
+        <v>2628555</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A23" s="18">
+        <v>1996</v>
+      </c>
+      <c r="B23">
+        <v>3696067</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A24" s="18">
+        <v>1997</v>
+      </c>
+      <c r="B24">
+        <v>4610042</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A25" s="18">
+        <v>1998</v>
+      </c>
+      <c r="B25">
+        <v>1902219</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A26" s="18">
+        <v>1999</v>
+      </c>
+      <c r="B26">
+        <v>2984568</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A27" s="18">
+        <v>2000</v>
+      </c>
+      <c r="B27">
+        <v>1814779</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A28" s="18">
+        <v>2001</v>
+      </c>
+      <c r="B28">
+        <v>2189670</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A29" s="18">
+        <v>2002</v>
+      </c>
+      <c r="B29">
+        <v>3466762</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A30" s="18">
+        <v>2003</v>
+      </c>
+      <c r="B30">
+        <v>4439571</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A31" s="18">
+        <v>2004</v>
+      </c>
+      <c r="B31">
+        <v>5705141</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A32" s="18">
+        <v>2005</v>
+      </c>
+      <c r="B32">
+        <v>6109173</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A33" s="18">
+        <v>2006</v>
+      </c>
+      <c r="B33">
+        <v>2848597</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A34" s="18">
+        <v>2007</v>
+      </c>
+      <c r="B34">
+        <v>3601777</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A35" s="18">
+        <v>2008</v>
+      </c>
+      <c r="B35">
+        <v>2082431</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A36" s="18">
+        <v>2009</v>
+      </c>
+      <c r="B36">
+        <v>2430414</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A37" s="18">
+        <v>2010</v>
+      </c>
+      <c r="B37">
+        <v>3596458</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A38" s="18">
+        <v>2011</v>
+      </c>
+      <c r="B38">
+        <v>6263091</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A39" s="18">
+        <v>2012</v>
+      </c>
+      <c r="B39">
+        <v>4769681</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A40" s="18">
+        <v>2013</v>
+      </c>
+      <c r="B40">
+        <v>3628121</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A41" s="18">
+        <v>2014</v>
+      </c>
+      <c r="B41">
+        <v>3404034</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A42" s="18">
+        <v>2015</v>
+      </c>
+      <c r="B42">
+        <v>3819016</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A43" s="18">
+        <v>2016</v>
+      </c>
+      <c r="B43">
+        <v>3711842</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A44" s="18">
+        <v>2017</v>
+      </c>
+      <c r="B44">
+        <v>2595720</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A45" s="18">
+        <v>2018</v>
+      </c>
+      <c r="B45">
+        <v>1867998</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A46" s="18">
+        <v>2019</v>
+      </c>
+      <c r="B46">
+        <v>3542442</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A47" s="18">
+        <v>2020</v>
+      </c>
+      <c r="B47">
+        <v>2394018</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A48" s="18">
+        <v>2021</v>
+      </c>
+      <c r="B48">
+        <v>3992341</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A49" s="18">
+        <v>2022</v>
+      </c>
+      <c r="B49">
+        <v>2929479</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A50" s="18">
+        <v>2023</v>
+      </c>
+      <c r="B50">
+        <v>3552933</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A51" s="18">
+        <v>2024</v>
+      </c>
+      <c r="B51">
+        <v>3724000</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A52" s="18"/>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A53" s="18"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>